<commit_message>
add error handling to setupfile
</commit_message>
<xml_diff>
--- a/test/plate_test_err.xlsx
+++ b/test/plate_test_err.xlsx
@@ -5,10 +5,13 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Ark2" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="Ark3" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="Ark4" sheetId="4" state="visible" r:id="rId5"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -20,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="13">
   <si>
     <t xml:space="preserve">Wnames</t>
   </si>
@@ -47,6 +50,18 @@
   </si>
   <si>
     <t xml:space="preserve">H</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I</t>
+  </si>
+  <si>
+    <t xml:space="preserve">J</t>
+  </si>
+  <si>
+    <t xml:space="preserve">K</t>
+  </si>
+  <si>
+    <t xml:space="preserve">L</t>
   </si>
 </sst>
 </file>
@@ -145,8 +160,8 @@
   </sheetPr>
   <dimension ref="A1:M10"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B10" activeCellId="0" sqref="B10:M10"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -681,4 +696,1488 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Side &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:M9"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="11.52"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C1" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D1" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="E1" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="F1" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="G1" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="H1" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="I1" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="J1" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="K1" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="L1" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="M1" s="0" t="n">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="0" t="str">
+        <f aca="false">$A2&amp;B$1</f>
+        <v>A1</v>
+      </c>
+      <c r="C2" s="0" t="str">
+        <f aca="false">$A2&amp;C$1</f>
+        <v>A1</v>
+      </c>
+      <c r="D2" s="0" t="str">
+        <f aca="false">$A2&amp;D$1</f>
+        <v>A3</v>
+      </c>
+      <c r="E2" s="0" t="str">
+        <f aca="false">$A2&amp;E$1</f>
+        <v>A4</v>
+      </c>
+      <c r="F2" s="0" t="str">
+        <f aca="false">$A2&amp;F$1</f>
+        <v>A5</v>
+      </c>
+      <c r="G2" s="0" t="str">
+        <f aca="false">$A2&amp;G$1</f>
+        <v>A6</v>
+      </c>
+      <c r="H2" s="0" t="str">
+        <f aca="false">$A2&amp;H$1</f>
+        <v>A7</v>
+      </c>
+      <c r="I2" s="0" t="str">
+        <f aca="false">$A2&amp;I$1</f>
+        <v>A8</v>
+      </c>
+      <c r="J2" s="0" t="str">
+        <f aca="false">$A2&amp;J$1</f>
+        <v>A9</v>
+      </c>
+      <c r="K2" s="0" t="str">
+        <f aca="false">$A2&amp;K$1</f>
+        <v>A10</v>
+      </c>
+      <c r="L2" s="0" t="str">
+        <f aca="false">$A2&amp;L$1</f>
+        <v>A11</v>
+      </c>
+      <c r="M2" s="0" t="str">
+        <f aca="false">$A2&amp;M$1</f>
+        <v>A12</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="0" t="str">
+        <f aca="false">$A3&amp;B$1</f>
+        <v>B1</v>
+      </c>
+      <c r="C3" s="0" t="str">
+        <f aca="false">$A3&amp;C$1</f>
+        <v>B1</v>
+      </c>
+      <c r="D3" s="0" t="str">
+        <f aca="false">$A3&amp;D$1</f>
+        <v>B3</v>
+      </c>
+      <c r="E3" s="0" t="str">
+        <f aca="false">$A3&amp;E$1</f>
+        <v>B4</v>
+      </c>
+      <c r="F3" s="0" t="str">
+        <f aca="false">$A3&amp;F$1</f>
+        <v>B5</v>
+      </c>
+      <c r="G3" s="0" t="str">
+        <f aca="false">$A3&amp;G$1</f>
+        <v>B6</v>
+      </c>
+      <c r="H3" s="0" t="str">
+        <f aca="false">$A3&amp;H$1</f>
+        <v>B7</v>
+      </c>
+      <c r="I3" s="0" t="str">
+        <f aca="false">$A3&amp;I$1</f>
+        <v>B8</v>
+      </c>
+      <c r="J3" s="0" t="str">
+        <f aca="false">$A3&amp;J$1</f>
+        <v>B9</v>
+      </c>
+      <c r="K3" s="0" t="str">
+        <f aca="false">$A3&amp;K$1</f>
+        <v>B10</v>
+      </c>
+      <c r="L3" s="0" t="str">
+        <f aca="false">$A3&amp;L$1</f>
+        <v>B11</v>
+      </c>
+      <c r="M3" s="0" t="str">
+        <f aca="false">$A3&amp;M$1</f>
+        <v>B12</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="0" t="str">
+        <f aca="false">$A4&amp;B$1</f>
+        <v>C1</v>
+      </c>
+      <c r="C4" s="0" t="str">
+        <f aca="false">$A4&amp;C$1</f>
+        <v>C1</v>
+      </c>
+      <c r="D4" s="0" t="str">
+        <f aca="false">$A4&amp;D$1</f>
+        <v>C3</v>
+      </c>
+      <c r="E4" s="0" t="str">
+        <f aca="false">$A4&amp;E$1</f>
+        <v>C4</v>
+      </c>
+      <c r="F4" s="0" t="str">
+        <f aca="false">$A4&amp;F$1</f>
+        <v>C5</v>
+      </c>
+      <c r="G4" s="0" t="str">
+        <f aca="false">$A4&amp;G$1</f>
+        <v>C6</v>
+      </c>
+      <c r="H4" s="0" t="str">
+        <f aca="false">$A4&amp;H$1</f>
+        <v>C7</v>
+      </c>
+      <c r="I4" s="0" t="str">
+        <f aca="false">$A4&amp;I$1</f>
+        <v>C8</v>
+      </c>
+      <c r="J4" s="0" t="str">
+        <f aca="false">$A4&amp;J$1</f>
+        <v>C9</v>
+      </c>
+      <c r="K4" s="0" t="str">
+        <f aca="false">$A4&amp;K$1</f>
+        <v>C10</v>
+      </c>
+      <c r="L4" s="0" t="str">
+        <f aca="false">$A4&amp;L$1</f>
+        <v>C11</v>
+      </c>
+      <c r="M4" s="0" t="str">
+        <f aca="false">$A4&amp;M$1</f>
+        <v>C12</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="0" t="str">
+        <f aca="false">$A5&amp;B$1</f>
+        <v>D1</v>
+      </c>
+      <c r="C5" s="0" t="str">
+        <f aca="false">$A5&amp;C$1</f>
+        <v>D1</v>
+      </c>
+      <c r="D5" s="0" t="str">
+        <f aca="false">$A5&amp;D$1</f>
+        <v>D3</v>
+      </c>
+      <c r="E5" s="0" t="str">
+        <f aca="false">$A5&amp;E$1</f>
+        <v>D4</v>
+      </c>
+      <c r="F5" s="0" t="str">
+        <f aca="false">$A5&amp;F$1</f>
+        <v>D5</v>
+      </c>
+      <c r="G5" s="0" t="str">
+        <f aca="false">$A5&amp;G$1</f>
+        <v>D6</v>
+      </c>
+      <c r="H5" s="0" t="str">
+        <f aca="false">$A5&amp;H$1</f>
+        <v>D7</v>
+      </c>
+      <c r="I5" s="0" t="str">
+        <f aca="false">$A5&amp;I$1</f>
+        <v>D8</v>
+      </c>
+      <c r="J5" s="0" t="str">
+        <f aca="false">$A5&amp;J$1</f>
+        <v>D9</v>
+      </c>
+      <c r="K5" s="0" t="str">
+        <f aca="false">$A5&amp;K$1</f>
+        <v>D10</v>
+      </c>
+      <c r="L5" s="0" t="str">
+        <f aca="false">$A5&amp;L$1</f>
+        <v>D11</v>
+      </c>
+      <c r="M5" s="0" t="str">
+        <f aca="false">$A5&amp;M$1</f>
+        <v>D12</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="0" t="str">
+        <f aca="false">$A6&amp;B$1</f>
+        <v>E1</v>
+      </c>
+      <c r="C6" s="0" t="str">
+        <f aca="false">$A6&amp;C$1</f>
+        <v>E1</v>
+      </c>
+      <c r="D6" s="0" t="str">
+        <f aca="false">$A6&amp;D$1</f>
+        <v>E3</v>
+      </c>
+      <c r="E6" s="0" t="str">
+        <f aca="false">$A6&amp;E$1</f>
+        <v>E4</v>
+      </c>
+      <c r="F6" s="0" t="str">
+        <f aca="false">$A6&amp;F$1</f>
+        <v>E5</v>
+      </c>
+      <c r="G6" s="0" t="str">
+        <f aca="false">$A6&amp;G$1</f>
+        <v>E6</v>
+      </c>
+      <c r="H6" s="0" t="str">
+        <f aca="false">$A6&amp;H$1</f>
+        <v>E7</v>
+      </c>
+      <c r="I6" s="0" t="str">
+        <f aca="false">$A6&amp;I$1</f>
+        <v>E8</v>
+      </c>
+      <c r="J6" s="0" t="str">
+        <f aca="false">$A6&amp;J$1</f>
+        <v>E9</v>
+      </c>
+      <c r="K6" s="0" t="str">
+        <f aca="false">$A6&amp;K$1</f>
+        <v>E10</v>
+      </c>
+      <c r="L6" s="0" t="str">
+        <f aca="false">$A6&amp;L$1</f>
+        <v>E11</v>
+      </c>
+      <c r="M6" s="0" t="str">
+        <f aca="false">$A6&amp;M$1</f>
+        <v>E12</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="0" t="str">
+        <f aca="false">$A7&amp;B$1</f>
+        <v>F1</v>
+      </c>
+      <c r="C7" s="0" t="str">
+        <f aca="false">$A7&amp;C$1</f>
+        <v>F1</v>
+      </c>
+      <c r="D7" s="0" t="str">
+        <f aca="false">$A7&amp;D$1</f>
+        <v>F3</v>
+      </c>
+      <c r="E7" s="0" t="str">
+        <f aca="false">$A7&amp;E$1</f>
+        <v>F4</v>
+      </c>
+      <c r="F7" s="0" t="str">
+        <f aca="false">$A7&amp;F$1</f>
+        <v>F5</v>
+      </c>
+      <c r="G7" s="0" t="str">
+        <f aca="false">$A7&amp;G$1</f>
+        <v>F6</v>
+      </c>
+      <c r="H7" s="0" t="str">
+        <f aca="false">$A7&amp;H$1</f>
+        <v>F7</v>
+      </c>
+      <c r="I7" s="0" t="str">
+        <f aca="false">$A7&amp;I$1</f>
+        <v>F8</v>
+      </c>
+      <c r="J7" s="0" t="str">
+        <f aca="false">$A7&amp;J$1</f>
+        <v>F9</v>
+      </c>
+      <c r="K7" s="0" t="str">
+        <f aca="false">$A7&amp;K$1</f>
+        <v>F10</v>
+      </c>
+      <c r="L7" s="0" t="str">
+        <f aca="false">$A7&amp;L$1</f>
+        <v>F11</v>
+      </c>
+      <c r="M7" s="0" t="str">
+        <f aca="false">$A7&amp;M$1</f>
+        <v>F12</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="0" t="str">
+        <f aca="false">$A8&amp;B$1</f>
+        <v>G1</v>
+      </c>
+      <c r="C8" s="0" t="str">
+        <f aca="false">$A8&amp;C$1</f>
+        <v>G1</v>
+      </c>
+      <c r="D8" s="0" t="str">
+        <f aca="false">$A8&amp;D$1</f>
+        <v>G3</v>
+      </c>
+      <c r="E8" s="0" t="str">
+        <f aca="false">$A8&amp;E$1</f>
+        <v>G4</v>
+      </c>
+      <c r="F8" s="0" t="str">
+        <f aca="false">$A8&amp;F$1</f>
+        <v>G5</v>
+      </c>
+      <c r="G8" s="0" t="str">
+        <f aca="false">$A8&amp;G$1</f>
+        <v>G6</v>
+      </c>
+      <c r="H8" s="0" t="str">
+        <f aca="false">$A8&amp;H$1</f>
+        <v>G7</v>
+      </c>
+      <c r="I8" s="0" t="str">
+        <f aca="false">$A8&amp;I$1</f>
+        <v>G8</v>
+      </c>
+      <c r="J8" s="0" t="str">
+        <f aca="false">$A8&amp;J$1</f>
+        <v>G9</v>
+      </c>
+      <c r="K8" s="0" t="str">
+        <f aca="false">$A8&amp;K$1</f>
+        <v>G10</v>
+      </c>
+      <c r="L8" s="0" t="str">
+        <f aca="false">$A8&amp;L$1</f>
+        <v>G11</v>
+      </c>
+      <c r="M8" s="0" t="str">
+        <f aca="false">$A8&amp;M$1</f>
+        <v>G12</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" s="0" t="str">
+        <f aca="false">$A9&amp;B$1</f>
+        <v>H1</v>
+      </c>
+      <c r="C9" s="0" t="str">
+        <f aca="false">$A9&amp;C$1</f>
+        <v>H1</v>
+      </c>
+      <c r="D9" s="0" t="str">
+        <f aca="false">$A9&amp;D$1</f>
+        <v>H3</v>
+      </c>
+      <c r="E9" s="0" t="str">
+        <f aca="false">$A9&amp;E$1</f>
+        <v>H4</v>
+      </c>
+      <c r="F9" s="0" t="str">
+        <f aca="false">$A9&amp;F$1</f>
+        <v>H5</v>
+      </c>
+      <c r="G9" s="0" t="str">
+        <f aca="false">$A9&amp;G$1</f>
+        <v>H6</v>
+      </c>
+      <c r="H9" s="0" t="str">
+        <f aca="false">$A9&amp;H$1</f>
+        <v>H7</v>
+      </c>
+      <c r="I9" s="0" t="str">
+        <f aca="false">$A9&amp;I$1</f>
+        <v>H8</v>
+      </c>
+      <c r="J9" s="0" t="str">
+        <f aca="false">$A9&amp;J$1</f>
+        <v>H9</v>
+      </c>
+      <c r="K9" s="0" t="str">
+        <f aca="false">$A9&amp;K$1</f>
+        <v>H10</v>
+      </c>
+      <c r="L9" s="0" t="str">
+        <f aca="false">$A9&amp;L$1</f>
+        <v>H11</v>
+      </c>
+      <c r="M9" s="0" t="str">
+        <f aca="false">$A9&amp;M$1</f>
+        <v>H12</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Side &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:M9"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="11.52"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C1" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="D1" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="E1" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="F1" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="G1" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="H1" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="I1" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="J1" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="K1" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="L1" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="M1" s="0" t="n">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="0" t="str">
+        <f aca="false">$A2&amp;B$1</f>
+        <v>A1</v>
+      </c>
+      <c r="C2" s="0" t="str">
+        <f aca="false">$A2&amp;C$1</f>
+        <v>A2</v>
+      </c>
+      <c r="D2" s="0" t="str">
+        <f aca="false">$A2&amp;D$1</f>
+        <v>A3</v>
+      </c>
+      <c r="E2" s="0" t="str">
+        <f aca="false">$A2&amp;E$1</f>
+        <v>A4</v>
+      </c>
+      <c r="F2" s="0" t="str">
+        <f aca="false">$A2&amp;F$1</f>
+        <v>A5</v>
+      </c>
+      <c r="G2" s="0" t="str">
+        <f aca="false">$A2&amp;G$1</f>
+        <v>A6</v>
+      </c>
+      <c r="H2" s="0" t="str">
+        <f aca="false">$A2&amp;H$1</f>
+        <v>A7</v>
+      </c>
+      <c r="I2" s="0" t="str">
+        <f aca="false">$A2&amp;I$1</f>
+        <v>A8</v>
+      </c>
+      <c r="J2" s="0" t="str">
+        <f aca="false">$A2&amp;J$1</f>
+        <v>A9</v>
+      </c>
+      <c r="K2" s="0" t="str">
+        <f aca="false">$A2&amp;K$1</f>
+        <v>A10</v>
+      </c>
+      <c r="L2" s="0" t="str">
+        <f aca="false">$A2&amp;L$1</f>
+        <v>A11</v>
+      </c>
+      <c r="M2" s="0" t="str">
+        <f aca="false">$A2&amp;M$1</f>
+        <v>A12</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="0" t="str">
+        <f aca="false">$A3&amp;B$1</f>
+        <v>A1</v>
+      </c>
+      <c r="C3" s="0" t="str">
+        <f aca="false">$A3&amp;C$1</f>
+        <v>A2</v>
+      </c>
+      <c r="D3" s="0" t="str">
+        <f aca="false">$A3&amp;D$1</f>
+        <v>A3</v>
+      </c>
+      <c r="E3" s="0" t="str">
+        <f aca="false">$A3&amp;E$1</f>
+        <v>A4</v>
+      </c>
+      <c r="F3" s="0" t="str">
+        <f aca="false">$A3&amp;F$1</f>
+        <v>A5</v>
+      </c>
+      <c r="G3" s="0" t="str">
+        <f aca="false">$A3&amp;G$1</f>
+        <v>A6</v>
+      </c>
+      <c r="H3" s="0" t="str">
+        <f aca="false">$A3&amp;H$1</f>
+        <v>A7</v>
+      </c>
+      <c r="I3" s="0" t="str">
+        <f aca="false">$A3&amp;I$1</f>
+        <v>A8</v>
+      </c>
+      <c r="J3" s="0" t="str">
+        <f aca="false">$A3&amp;J$1</f>
+        <v>A9</v>
+      </c>
+      <c r="K3" s="0" t="str">
+        <f aca="false">$A3&amp;K$1</f>
+        <v>A10</v>
+      </c>
+      <c r="L3" s="0" t="str">
+        <f aca="false">$A3&amp;L$1</f>
+        <v>A11</v>
+      </c>
+      <c r="M3" s="0" t="str">
+        <f aca="false">$A3&amp;M$1</f>
+        <v>A12</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="0" t="str">
+        <f aca="false">$A4&amp;B$1</f>
+        <v>C1</v>
+      </c>
+      <c r="C4" s="0" t="str">
+        <f aca="false">$A4&amp;C$1</f>
+        <v>C2</v>
+      </c>
+      <c r="D4" s="0" t="str">
+        <f aca="false">$A4&amp;D$1</f>
+        <v>C3</v>
+      </c>
+      <c r="E4" s="0" t="str">
+        <f aca="false">$A4&amp;E$1</f>
+        <v>C4</v>
+      </c>
+      <c r="F4" s="0" t="str">
+        <f aca="false">$A4&amp;F$1</f>
+        <v>C5</v>
+      </c>
+      <c r="G4" s="0" t="str">
+        <f aca="false">$A4&amp;G$1</f>
+        <v>C6</v>
+      </c>
+      <c r="H4" s="0" t="str">
+        <f aca="false">$A4&amp;H$1</f>
+        <v>C7</v>
+      </c>
+      <c r="I4" s="0" t="str">
+        <f aca="false">$A4&amp;I$1</f>
+        <v>C8</v>
+      </c>
+      <c r="J4" s="0" t="str">
+        <f aca="false">$A4&amp;J$1</f>
+        <v>C9</v>
+      </c>
+      <c r="K4" s="0" t="str">
+        <f aca="false">$A4&amp;K$1</f>
+        <v>C10</v>
+      </c>
+      <c r="L4" s="0" t="str">
+        <f aca="false">$A4&amp;L$1</f>
+        <v>C11</v>
+      </c>
+      <c r="M4" s="0" t="str">
+        <f aca="false">$A4&amp;M$1</f>
+        <v>C12</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="0" t="str">
+        <f aca="false">$A5&amp;B$1</f>
+        <v>D1</v>
+      </c>
+      <c r="C5" s="0" t="str">
+        <f aca="false">$A5&amp;C$1</f>
+        <v>D2</v>
+      </c>
+      <c r="D5" s="0" t="str">
+        <f aca="false">$A5&amp;D$1</f>
+        <v>D3</v>
+      </c>
+      <c r="E5" s="0" t="str">
+        <f aca="false">$A5&amp;E$1</f>
+        <v>D4</v>
+      </c>
+      <c r="F5" s="0" t="str">
+        <f aca="false">$A5&amp;F$1</f>
+        <v>D5</v>
+      </c>
+      <c r="G5" s="0" t="str">
+        <f aca="false">$A5&amp;G$1</f>
+        <v>D6</v>
+      </c>
+      <c r="H5" s="0" t="str">
+        <f aca="false">$A5&amp;H$1</f>
+        <v>D7</v>
+      </c>
+      <c r="I5" s="0" t="str">
+        <f aca="false">$A5&amp;I$1</f>
+        <v>D8</v>
+      </c>
+      <c r="J5" s="0" t="str">
+        <f aca="false">$A5&amp;J$1</f>
+        <v>D9</v>
+      </c>
+      <c r="K5" s="0" t="str">
+        <f aca="false">$A5&amp;K$1</f>
+        <v>D10</v>
+      </c>
+      <c r="L5" s="0" t="str">
+        <f aca="false">$A5&amp;L$1</f>
+        <v>D11</v>
+      </c>
+      <c r="M5" s="0" t="str">
+        <f aca="false">$A5&amp;M$1</f>
+        <v>D12</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="0" t="str">
+        <f aca="false">$A6&amp;B$1</f>
+        <v>E1</v>
+      </c>
+      <c r="C6" s="0" t="str">
+        <f aca="false">$A6&amp;C$1</f>
+        <v>E2</v>
+      </c>
+      <c r="D6" s="0" t="str">
+        <f aca="false">$A6&amp;D$1</f>
+        <v>E3</v>
+      </c>
+      <c r="E6" s="0" t="str">
+        <f aca="false">$A6&amp;E$1</f>
+        <v>E4</v>
+      </c>
+      <c r="F6" s="0" t="str">
+        <f aca="false">$A6&amp;F$1</f>
+        <v>E5</v>
+      </c>
+      <c r="G6" s="0" t="str">
+        <f aca="false">$A6&amp;G$1</f>
+        <v>E6</v>
+      </c>
+      <c r="H6" s="0" t="str">
+        <f aca="false">$A6&amp;H$1</f>
+        <v>E7</v>
+      </c>
+      <c r="I6" s="0" t="str">
+        <f aca="false">$A6&amp;I$1</f>
+        <v>E8</v>
+      </c>
+      <c r="J6" s="0" t="str">
+        <f aca="false">$A6&amp;J$1</f>
+        <v>E9</v>
+      </c>
+      <c r="K6" s="0" t="str">
+        <f aca="false">$A6&amp;K$1</f>
+        <v>E10</v>
+      </c>
+      <c r="L6" s="0" t="str">
+        <f aca="false">$A6&amp;L$1</f>
+        <v>E11</v>
+      </c>
+      <c r="M6" s="0" t="str">
+        <f aca="false">$A6&amp;M$1</f>
+        <v>E12</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="0" t="str">
+        <f aca="false">$A7&amp;B$1</f>
+        <v>F1</v>
+      </c>
+      <c r="C7" s="0" t="str">
+        <f aca="false">$A7&amp;C$1</f>
+        <v>F2</v>
+      </c>
+      <c r="D7" s="0" t="str">
+        <f aca="false">$A7&amp;D$1</f>
+        <v>F3</v>
+      </c>
+      <c r="E7" s="0" t="str">
+        <f aca="false">$A7&amp;E$1</f>
+        <v>F4</v>
+      </c>
+      <c r="F7" s="0" t="str">
+        <f aca="false">$A7&amp;F$1</f>
+        <v>F5</v>
+      </c>
+      <c r="G7" s="0" t="str">
+        <f aca="false">$A7&amp;G$1</f>
+        <v>F6</v>
+      </c>
+      <c r="H7" s="0" t="str">
+        <f aca="false">$A7&amp;H$1</f>
+        <v>F7</v>
+      </c>
+      <c r="I7" s="0" t="str">
+        <f aca="false">$A7&amp;I$1</f>
+        <v>F8</v>
+      </c>
+      <c r="J7" s="0" t="str">
+        <f aca="false">$A7&amp;J$1</f>
+        <v>F9</v>
+      </c>
+      <c r="K7" s="0" t="str">
+        <f aca="false">$A7&amp;K$1</f>
+        <v>F10</v>
+      </c>
+      <c r="L7" s="0" t="str">
+        <f aca="false">$A7&amp;L$1</f>
+        <v>F11</v>
+      </c>
+      <c r="M7" s="0" t="str">
+        <f aca="false">$A7&amp;M$1</f>
+        <v>F12</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="0" t="str">
+        <f aca="false">$A8&amp;B$1</f>
+        <v>G1</v>
+      </c>
+      <c r="C8" s="0" t="str">
+        <f aca="false">$A8&amp;C$1</f>
+        <v>G2</v>
+      </c>
+      <c r="D8" s="0" t="str">
+        <f aca="false">$A8&amp;D$1</f>
+        <v>G3</v>
+      </c>
+      <c r="E8" s="0" t="str">
+        <f aca="false">$A8&amp;E$1</f>
+        <v>G4</v>
+      </c>
+      <c r="F8" s="0" t="str">
+        <f aca="false">$A8&amp;F$1</f>
+        <v>G5</v>
+      </c>
+      <c r="G8" s="0" t="str">
+        <f aca="false">$A8&amp;G$1</f>
+        <v>G6</v>
+      </c>
+      <c r="H8" s="0" t="str">
+        <f aca="false">$A8&amp;H$1</f>
+        <v>G7</v>
+      </c>
+      <c r="I8" s="0" t="str">
+        <f aca="false">$A8&amp;I$1</f>
+        <v>G8</v>
+      </c>
+      <c r="J8" s="0" t="str">
+        <f aca="false">$A8&amp;J$1</f>
+        <v>G9</v>
+      </c>
+      <c r="K8" s="0" t="str">
+        <f aca="false">$A8&amp;K$1</f>
+        <v>G10</v>
+      </c>
+      <c r="L8" s="0" t="str">
+        <f aca="false">$A8&amp;L$1</f>
+        <v>G11</v>
+      </c>
+      <c r="M8" s="0" t="str">
+        <f aca="false">$A8&amp;M$1</f>
+        <v>G12</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" s="0" t="str">
+        <f aca="false">$A9&amp;B$1</f>
+        <v>H1</v>
+      </c>
+      <c r="C9" s="0" t="str">
+        <f aca="false">$A9&amp;C$1</f>
+        <v>H2</v>
+      </c>
+      <c r="D9" s="0" t="str">
+        <f aca="false">$A9&amp;D$1</f>
+        <v>H3</v>
+      </c>
+      <c r="E9" s="0" t="str">
+        <f aca="false">$A9&amp;E$1</f>
+        <v>H4</v>
+      </c>
+      <c r="F9" s="0" t="str">
+        <f aca="false">$A9&amp;F$1</f>
+        <v>H5</v>
+      </c>
+      <c r="G9" s="0" t="str">
+        <f aca="false">$A9&amp;G$1</f>
+        <v>H6</v>
+      </c>
+      <c r="H9" s="0" t="str">
+        <f aca="false">$A9&amp;H$1</f>
+        <v>H7</v>
+      </c>
+      <c r="I9" s="0" t="str">
+        <f aca="false">$A9&amp;I$1</f>
+        <v>H8</v>
+      </c>
+      <c r="J9" s="0" t="str">
+        <f aca="false">$A9&amp;J$1</f>
+        <v>H9</v>
+      </c>
+      <c r="K9" s="0" t="str">
+        <f aca="false">$A9&amp;K$1</f>
+        <v>H10</v>
+      </c>
+      <c r="L9" s="0" t="str">
+        <f aca="false">$A9&amp;L$1</f>
+        <v>H11</v>
+      </c>
+      <c r="M9" s="0" t="str">
+        <f aca="false">$A9&amp;M$1</f>
+        <v>H12</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Side &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:I13"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B12" activeCellId="0" sqref="B12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="11.52"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C1" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="D1" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="E1" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="F1" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="G1" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="H1" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="I1" s="0" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="0" t="str">
+        <f aca="false">$A2&amp;B$1</f>
+        <v>A1</v>
+      </c>
+      <c r="C2" s="0" t="str">
+        <f aca="false">$A2&amp;C$1</f>
+        <v>A2</v>
+      </c>
+      <c r="D2" s="0" t="str">
+        <f aca="false">$A2&amp;D$1</f>
+        <v>A3</v>
+      </c>
+      <c r="E2" s="0" t="str">
+        <f aca="false">$A2&amp;E$1</f>
+        <v>A4</v>
+      </c>
+      <c r="F2" s="0" t="str">
+        <f aca="false">$A2&amp;F$1</f>
+        <v>A5</v>
+      </c>
+      <c r="G2" s="0" t="str">
+        <f aca="false">$A2&amp;G$1</f>
+        <v>A6</v>
+      </c>
+      <c r="H2" s="0" t="str">
+        <f aca="false">$A2&amp;H$1</f>
+        <v>A7</v>
+      </c>
+      <c r="I2" s="0" t="str">
+        <f aca="false">$A2&amp;I$1</f>
+        <v>A8</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="0" t="str">
+        <f aca="false">$A3&amp;B$1</f>
+        <v>B1</v>
+      </c>
+      <c r="C3" s="0" t="str">
+        <f aca="false">$A3&amp;C$1</f>
+        <v>B2</v>
+      </c>
+      <c r="D3" s="0" t="str">
+        <f aca="false">$A3&amp;D$1</f>
+        <v>B3</v>
+      </c>
+      <c r="E3" s="0" t="str">
+        <f aca="false">$A3&amp;E$1</f>
+        <v>B4</v>
+      </c>
+      <c r="F3" s="0" t="str">
+        <f aca="false">$A3&amp;F$1</f>
+        <v>B5</v>
+      </c>
+      <c r="G3" s="0" t="str">
+        <f aca="false">$A3&amp;G$1</f>
+        <v>B6</v>
+      </c>
+      <c r="H3" s="0" t="str">
+        <f aca="false">$A3&amp;H$1</f>
+        <v>B7</v>
+      </c>
+      <c r="I3" s="0" t="str">
+        <f aca="false">$A3&amp;I$1</f>
+        <v>B8</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="0" t="str">
+        <f aca="false">$A4&amp;B$1</f>
+        <v>C1</v>
+      </c>
+      <c r="C4" s="0" t="str">
+        <f aca="false">$A4&amp;C$1</f>
+        <v>C2</v>
+      </c>
+      <c r="D4" s="0" t="str">
+        <f aca="false">$A4&amp;D$1</f>
+        <v>C3</v>
+      </c>
+      <c r="E4" s="0" t="str">
+        <f aca="false">$A4&amp;E$1</f>
+        <v>C4</v>
+      </c>
+      <c r="F4" s="0" t="str">
+        <f aca="false">$A4&amp;F$1</f>
+        <v>C5</v>
+      </c>
+      <c r="G4" s="0" t="str">
+        <f aca="false">$A4&amp;G$1</f>
+        <v>C6</v>
+      </c>
+      <c r="H4" s="0" t="str">
+        <f aca="false">$A4&amp;H$1</f>
+        <v>C7</v>
+      </c>
+      <c r="I4" s="0" t="str">
+        <f aca="false">$A4&amp;I$1</f>
+        <v>C8</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="0" t="str">
+        <f aca="false">$A5&amp;B$1</f>
+        <v>D1</v>
+      </c>
+      <c r="C5" s="0" t="str">
+        <f aca="false">$A5&amp;C$1</f>
+        <v>D2</v>
+      </c>
+      <c r="D5" s="0" t="str">
+        <f aca="false">$A5&amp;D$1</f>
+        <v>D3</v>
+      </c>
+      <c r="E5" s="0" t="str">
+        <f aca="false">$A5&amp;E$1</f>
+        <v>D4</v>
+      </c>
+      <c r="F5" s="0" t="str">
+        <f aca="false">$A5&amp;F$1</f>
+        <v>D5</v>
+      </c>
+      <c r="G5" s="0" t="str">
+        <f aca="false">$A5&amp;G$1</f>
+        <v>D6</v>
+      </c>
+      <c r="H5" s="0" t="str">
+        <f aca="false">$A5&amp;H$1</f>
+        <v>D7</v>
+      </c>
+      <c r="I5" s="0" t="str">
+        <f aca="false">$A5&amp;I$1</f>
+        <v>D8</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="0" t="str">
+        <f aca="false">$A6&amp;B$1</f>
+        <v>E1</v>
+      </c>
+      <c r="C6" s="0" t="str">
+        <f aca="false">$A6&amp;C$1</f>
+        <v>E2</v>
+      </c>
+      <c r="D6" s="0" t="str">
+        <f aca="false">$A6&amp;D$1</f>
+        <v>E3</v>
+      </c>
+      <c r="E6" s="0" t="str">
+        <f aca="false">$A6&amp;E$1</f>
+        <v>E4</v>
+      </c>
+      <c r="F6" s="0" t="str">
+        <f aca="false">$A6&amp;F$1</f>
+        <v>E5</v>
+      </c>
+      <c r="G6" s="0" t="str">
+        <f aca="false">$A6&amp;G$1</f>
+        <v>E6</v>
+      </c>
+      <c r="H6" s="0" t="str">
+        <f aca="false">$A6&amp;H$1</f>
+        <v>E7</v>
+      </c>
+      <c r="I6" s="0" t="str">
+        <f aca="false">$A6&amp;I$1</f>
+        <v>E8</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="0" t="str">
+        <f aca="false">$A7&amp;B$1</f>
+        <v>F1</v>
+      </c>
+      <c r="C7" s="0" t="str">
+        <f aca="false">$A7&amp;C$1</f>
+        <v>F2</v>
+      </c>
+      <c r="D7" s="0" t="str">
+        <f aca="false">$A7&amp;D$1</f>
+        <v>F3</v>
+      </c>
+      <c r="E7" s="0" t="str">
+        <f aca="false">$A7&amp;E$1</f>
+        <v>F4</v>
+      </c>
+      <c r="F7" s="0" t="str">
+        <f aca="false">$A7&amp;F$1</f>
+        <v>F5</v>
+      </c>
+      <c r="G7" s="0" t="str">
+        <f aca="false">$A7&amp;G$1</f>
+        <v>F6</v>
+      </c>
+      <c r="H7" s="0" t="str">
+        <f aca="false">$A7&amp;H$1</f>
+        <v>F7</v>
+      </c>
+      <c r="I7" s="0" t="str">
+        <f aca="false">$A7&amp;I$1</f>
+        <v>F8</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="0" t="str">
+        <f aca="false">$A8&amp;B$1</f>
+        <v>G1</v>
+      </c>
+      <c r="C8" s="0" t="str">
+        <f aca="false">$A8&amp;C$1</f>
+        <v>G2</v>
+      </c>
+      <c r="D8" s="0" t="str">
+        <f aca="false">$A8&amp;D$1</f>
+        <v>G3</v>
+      </c>
+      <c r="E8" s="0" t="str">
+        <f aca="false">$A8&amp;E$1</f>
+        <v>G4</v>
+      </c>
+      <c r="F8" s="0" t="str">
+        <f aca="false">$A8&amp;F$1</f>
+        <v>G5</v>
+      </c>
+      <c r="G8" s="0" t="str">
+        <f aca="false">$A8&amp;G$1</f>
+        <v>G6</v>
+      </c>
+      <c r="H8" s="0" t="str">
+        <f aca="false">$A8&amp;H$1</f>
+        <v>G7</v>
+      </c>
+      <c r="I8" s="0" t="str">
+        <f aca="false">$A8&amp;I$1</f>
+        <v>G8</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" s="0" t="str">
+        <f aca="false">$A9&amp;B$1</f>
+        <v>H1</v>
+      </c>
+      <c r="C9" s="0" t="str">
+        <f aca="false">$A9&amp;C$1</f>
+        <v>H2</v>
+      </c>
+      <c r="D9" s="0" t="str">
+        <f aca="false">$A9&amp;D$1</f>
+        <v>H3</v>
+      </c>
+      <c r="E9" s="0" t="str">
+        <f aca="false">$A9&amp;E$1</f>
+        <v>H4</v>
+      </c>
+      <c r="F9" s="0" t="str">
+        <f aca="false">$A9&amp;F$1</f>
+        <v>H5</v>
+      </c>
+      <c r="G9" s="0" t="str">
+        <f aca="false">$A9&amp;G$1</f>
+        <v>H6</v>
+      </c>
+      <c r="H9" s="0" t="str">
+        <f aca="false">$A9&amp;H$1</f>
+        <v>H7</v>
+      </c>
+      <c r="I9" s="0" t="str">
+        <f aca="false">$A9&amp;I$1</f>
+        <v>H8</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" s="0" t="str">
+        <f aca="false">$A10&amp;B$1</f>
+        <v>I1</v>
+      </c>
+      <c r="C10" s="0" t="str">
+        <f aca="false">$A10&amp;C$1</f>
+        <v>I2</v>
+      </c>
+      <c r="D10" s="0" t="str">
+        <f aca="false">$A10&amp;D$1</f>
+        <v>I3</v>
+      </c>
+      <c r="E10" s="0" t="str">
+        <f aca="false">$A10&amp;E$1</f>
+        <v>I4</v>
+      </c>
+      <c r="F10" s="0" t="str">
+        <f aca="false">$A10&amp;F$1</f>
+        <v>I5</v>
+      </c>
+      <c r="G10" s="0" t="str">
+        <f aca="false">$A10&amp;G$1</f>
+        <v>I6</v>
+      </c>
+      <c r="H10" s="0" t="str">
+        <f aca="false">$A10&amp;H$1</f>
+        <v>I7</v>
+      </c>
+      <c r="I10" s="0" t="str">
+        <f aca="false">$A10&amp;I$1</f>
+        <v>I8</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11" s="0" t="str">
+        <f aca="false">$A11&amp;B$1</f>
+        <v>J1</v>
+      </c>
+      <c r="C11" s="0" t="str">
+        <f aca="false">$A11&amp;C$1</f>
+        <v>J2</v>
+      </c>
+      <c r="D11" s="0" t="str">
+        <f aca="false">$A11&amp;D$1</f>
+        <v>J3</v>
+      </c>
+      <c r="E11" s="0" t="str">
+        <f aca="false">$A11&amp;E$1</f>
+        <v>J4</v>
+      </c>
+      <c r="F11" s="0" t="str">
+        <f aca="false">$A11&amp;F$1</f>
+        <v>J5</v>
+      </c>
+      <c r="G11" s="0" t="str">
+        <f aca="false">$A11&amp;G$1</f>
+        <v>J6</v>
+      </c>
+      <c r="H11" s="0" t="str">
+        <f aca="false">$A11&amp;H$1</f>
+        <v>J7</v>
+      </c>
+      <c r="I11" s="0" t="str">
+        <f aca="false">$A11&amp;I$1</f>
+        <v>J8</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12" s="0" t="str">
+        <f aca="false">$A12&amp;B$1</f>
+        <v>K1</v>
+      </c>
+      <c r="C12" s="0" t="str">
+        <f aca="false">$A12&amp;C$1</f>
+        <v>K2</v>
+      </c>
+      <c r="D12" s="0" t="str">
+        <f aca="false">$A12&amp;D$1</f>
+        <v>K3</v>
+      </c>
+      <c r="E12" s="0" t="str">
+        <f aca="false">$A12&amp;E$1</f>
+        <v>K4</v>
+      </c>
+      <c r="F12" s="0" t="str">
+        <f aca="false">$A12&amp;F$1</f>
+        <v>K5</v>
+      </c>
+      <c r="G12" s="0" t="str">
+        <f aca="false">$A12&amp;G$1</f>
+        <v>K6</v>
+      </c>
+      <c r="H12" s="0" t="str">
+        <f aca="false">$A12&amp;H$1</f>
+        <v>K7</v>
+      </c>
+      <c r="I12" s="0" t="str">
+        <f aca="false">$A12&amp;I$1</f>
+        <v>K8</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="B13" s="0" t="str">
+        <f aca="false">$A13&amp;B$1</f>
+        <v>L1</v>
+      </c>
+      <c r="C13" s="0" t="str">
+        <f aca="false">$A13&amp;C$1</f>
+        <v>L2</v>
+      </c>
+      <c r="D13" s="0" t="str">
+        <f aca="false">$A13&amp;D$1</f>
+        <v>L3</v>
+      </c>
+      <c r="E13" s="0" t="str">
+        <f aca="false">$A13&amp;E$1</f>
+        <v>L4</v>
+      </c>
+      <c r="F13" s="0" t="str">
+        <f aca="false">$A13&amp;F$1</f>
+        <v>L5</v>
+      </c>
+      <c r="G13" s="0" t="str">
+        <f aca="false">$A13&amp;G$1</f>
+        <v>L6</v>
+      </c>
+      <c r="H13" s="0" t="str">
+        <f aca="false">$A13&amp;H$1</f>
+        <v>L7</v>
+      </c>
+      <c r="I13" s="0" t="str">
+        <f aca="false">$A13&amp;I$1</f>
+        <v>L8</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Side &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>